<commit_message>
Adding basic extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janko\eclipse-workspace\NopCommerceV1\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janko\git\projects\NopCommerce\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9502A81-E1B9-45AC-BA64-6DAEA9764D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1282647-2598-40B0-BC37-E839C84D38DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="register" sheetId="2" r:id="rId2"/>
+    <sheet name="register" sheetId="2" r:id="rId1"/>
+    <sheet name="login" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>password</t>
   </si>
@@ -43,32 +43,14 @@
     <t>testemail</t>
   </si>
   <si>
-    <t>random2@gmail.com</t>
-  </si>
-  <si>
-    <t>random3@gmail.com</t>
-  </si>
-  <si>
-    <t>random4@gmail.com</t>
-  </si>
-  <si>
-    <t>random4</t>
-  </si>
-  <si>
     <t>random1</t>
-  </si>
-  <si>
-    <t>random2</t>
-  </si>
-  <si>
-    <t>random3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,12 +62,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -395,84 +371,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="18.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{3E2D0818-05C5-4EB2-9BA2-F9D065A72FD0}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{6182D3F9-2A4C-48E7-9CF7-595498F5EA3F}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{35994B0F-EEBF-42A9-BB50-D27F99D81070}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{59E4D25A-B083-43C5-B3BC-81723E0AF048}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{33161802-6A8B-45F1-9845-693AC2E23683}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481FC869-B538-429F-9D05-691247D8EB6D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
@@ -512,4 +414,50 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350F98E2-093F-4A42-9A48-CDBD8083FF05}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{35571645-67AB-44A0-BA5A-9BE7C1DF067E}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{ACA81296-603D-44C1-851C-37024FFFB50F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding registration functionality test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janko\git\projects\NopCommerce\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1282647-2598-40B0-BC37-E839C84D38DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF7783F-D77C-42A5-BE66-63ADC065A0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="736" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="2" r:id="rId1"/>
     <sheet name="login" sheetId="3" r:id="rId2"/>
+    <sheet name="TC_RF_001" sheetId="4" r:id="rId3"/>
+    <sheet name="TC_RF_002" sheetId="5" r:id="rId4"/>
+    <sheet name="TC_RF_005" sheetId="6" r:id="rId5"/>
+    <sheet name="TC_RF_006" sheetId="7" r:id="rId6"/>
+    <sheet name="TC_RF_007" sheetId="8" r:id="rId7"/>
+    <sheet name="TC_RF_008" sheetId="9" r:id="rId8"/>
+    <sheet name="TC_RF_009" sheetId="10" r:id="rId9"/>
+    <sheet name="TC_RF_010" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="29">
   <si>
     <t>password</t>
   </si>
@@ -44,6 +52,75 @@
   </si>
   <si>
     <t>random1</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm password</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Bourne</t>
+  </si>
+  <si>
+    <t>jasonb@gmail.com</t>
+  </si>
+  <si>
+    <t>jasonb</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>johns@gmail.com</t>
+  </si>
+  <si>
+    <t>johnsmith</t>
+  </si>
+  <si>
+    <t>jasonb5@gmail.com</t>
+  </si>
+  <si>
+    <t>jasonb5</t>
+  </si>
+  <si>
+    <t>jasonb65@gmail.com</t>
+  </si>
+  <si>
+    <t>jasonb8</t>
+  </si>
+  <si>
+    <t>jasonb8@</t>
+  </si>
+  <si>
+    <t>jasonb8@gmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t>jasonb10@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -375,52 +452,6 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="18.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{5544651A-887F-45C6-B1B4-60CC2FD5E90C}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{0307BF96-C785-4023-BE46-092A63FB8882}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350F98E2-093F-4A42-9A48-CDBD8083FF05}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -439,6 +470,107 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5544651A-887F-45C6-B1B4-60CC2FD5E90C}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{0307BF96-C785-4023-BE46-092A63FB8882}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45E70C2-2940-4927-949B-F4E73326306F}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2">
+        <v>123</v>
+      </c>
+      <c r="E2">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{DA06FB96-C517-4288-838F-DFA74A593612}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350F98E2-093F-4A42-9A48-CDBD8083FF05}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -460,4 +592,422 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CCC1BC-0734-453D-9B53-074DBEFD9887}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5A27E0AF-10A5-4C7B-81FB-8F1DECFA1514}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFFC51EA-31EC-45BE-935D-C8EB3A636EAE}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A9AC1603-6FF0-40E5-8D94-146FAF5527EE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD92261-744C-4231-A527-2E5E9A1CBE56}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{D19C3392-A373-41C7-A31B-0D9D0364C7DD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E246198-FBB2-4378-8B9E-C4EC2F24E7A6}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{EBA57591-CE75-4215-B115-99BA6B56274C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B4CB84-7155-455D-9348-FBB9F3687F3C}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{24910ED5-2E22-46DE-B919-E4E51A718D2D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7187849E-93D2-4216-8FD0-A81D6FD93674}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="jasonb@gmail.com" xr:uid="{2049C5DD-1351-4615-B760-11227F2F14C0}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{7D57F314-9378-4A2D-B066-992AF2C94719}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{7E014B4C-FBD1-48B6-A03D-68D498700E88}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F42AFF-70F5-4FDB-9AA4-AB18D142B6B4}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="jasonb@gmail.com" xr:uid="{4BF6B43B-AB38-453A-9D63-F2EBDAAC9A6C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adjustments and adding manual testing
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janko\git\projects\NopCommerce\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF7783F-D77C-42A5-BE66-63ADC065A0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0104A8B1-91A6-4BD2-B322-F47D120A96FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="736" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="736" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="register" sheetId="2" r:id="rId1"/>
-    <sheet name="login" sheetId="3" r:id="rId2"/>
-    <sheet name="TC_RF_001" sheetId="4" r:id="rId3"/>
-    <sheet name="TC_RF_002" sheetId="5" r:id="rId4"/>
-    <sheet name="TC_RF_005" sheetId="6" r:id="rId5"/>
-    <sheet name="TC_RF_006" sheetId="7" r:id="rId6"/>
-    <sheet name="TC_RF_007" sheetId="8" r:id="rId7"/>
-    <sheet name="TC_RF_008" sheetId="9" r:id="rId8"/>
-    <sheet name="TC_RF_009" sheetId="10" r:id="rId9"/>
-    <sheet name="TC_RF_010" sheetId="11" r:id="rId10"/>
+    <sheet name="TC_RF_001" sheetId="4" r:id="rId1"/>
+    <sheet name="TC_RF_002" sheetId="5" r:id="rId2"/>
+    <sheet name="TC_RF_004" sheetId="6" r:id="rId3"/>
+    <sheet name="TC_RF_005" sheetId="7" r:id="rId4"/>
+    <sheet name="TC_RF_006" sheetId="8" r:id="rId5"/>
+    <sheet name="TC_RF_007" sheetId="9" r:id="rId6"/>
+    <sheet name="TC_RF_008" sheetId="14" r:id="rId7"/>
+    <sheet name="TC_RF_009" sheetId="11" r:id="rId8"/>
+    <sheet name="TC_LF_002" sheetId="12" r:id="rId9"/>
+    <sheet name="TC_LF_003" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,25 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="29">
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>testemail@gmail.com</t>
-  </si>
-  <si>
-    <t>random1@gmail.com</t>
-  </si>
-  <si>
-    <t>testemail</t>
-  </si>
-  <si>
-    <t>random1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="22">
   <si>
     <t>First name</t>
   </si>
@@ -93,34 +75,31 @@
     <t>johnsmith</t>
   </si>
   <si>
-    <t>jasonb5@gmail.com</t>
-  </si>
-  <si>
     <t>jasonb5</t>
   </si>
   <si>
-    <t>jasonb65@gmail.com</t>
-  </si>
-  <si>
-    <t>jasonb8</t>
-  </si>
-  <si>
-    <t>jasonb8@</t>
-  </si>
-  <si>
-    <t>jasonb8@gmail</t>
-  </si>
-  <si>
     <t xml:space="preserve">      </t>
   </si>
   <si>
-    <t xml:space="preserve">       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        </t>
-  </si>
-  <si>
-    <t>jasonb10@gmail.com</t>
+    <t>lukes2@gmail.com</t>
+  </si>
+  <si>
+    <t>jasonb4@gmail.com</t>
+  </si>
+  <si>
+    <t>jasonb54@gmail.com</t>
+  </si>
+  <si>
+    <t>jasonb7</t>
+  </si>
+  <si>
+    <t>jasonb7@</t>
+  </si>
+  <si>
+    <t>jasonb7@gmail</t>
+  </si>
+  <si>
+    <t>jasonb9@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -448,11 +427,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481FC869-B538-429F-9D05-691247D8EB6D}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CCC1BC-0734-453D-9B53-074DBEFD9887}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5A27E0AF-10A5-4C7B-81FB-8F1DECFA1514}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60C0F3B-A43B-408B-A2B3-130BAD8DE336}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,194 +496,29 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>987123</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{5544651A-887F-45C6-B1B4-60CC2FD5E90C}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{0307BF96-C785-4023-BE46-092A63FB8882}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{63F060E4-0D38-4C14-A1C7-1FA5D1FB0381}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45E70C2-2940-4927-949B-F4E73326306F}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="5" width="18.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2">
-        <v>123</v>
-      </c>
-      <c r="E2">
-        <v>123</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{DA06FB96-C517-4288-838F-DFA74A593612}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350F98E2-093F-4A42-9A48-CDBD8083FF05}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="18.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{35571645-67AB-44A0-BA5A-9BE7C1DF067E}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{ACA81296-603D-44C1-851C-37024FFFB50F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CCC1BC-0734-453D-9B53-074DBEFD9887}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="5" width="18.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{5A27E0AF-10A5-4C7B-81FB-8F1DECFA1514}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFFC51EA-31EC-45BE-935D-C8EB3A636EAE}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -664,36 +533,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -704,7 +573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD92261-744C-4231-A527-2E5E9A1CBE56}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -719,36 +588,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -759,12 +628,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E246198-FBB2-4378-8B9E-C4EC2F24E7A6}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -774,33 +643,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -811,8 +680,154 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B4CB84-7155-455D-9348-FBB9F3687F3C}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{3B188DEB-D0A5-4FA3-B662-138EEDB8D69A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7187849E-93D2-4216-8FD0-A81D6FD93674}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="jasonb@gmail.com" xr:uid="{2049C5DD-1351-4615-B760-11227F2F14C0}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{7D57F314-9378-4A2D-B066-992AF2C94719}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{7E014B4C-FBD1-48B6-A03D-68D498700E88}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B4CB84-7155-455D-9348-FBB9F3687F3C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892B2189-27F9-438E-932A-EB6DCA489321}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -826,30 +841,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -860,18 +875,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{24910ED5-2E22-46DE-B919-E4E51A718D2D}"/>
+    <hyperlink ref="C2" r:id="rId1" display="jasonb@gmail.com" xr:uid="{BD3DB3B5-9E68-49DF-8947-FAB263790BA2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7187849E-93D2-4216-8FD0-A81D6FD93674}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45E70C2-2940-4927-949B-F4E73326306F}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,132 +896,78 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>123</v>
+      </c>
+      <c r="E2">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="jasonb@gmail.com" xr:uid="{2049C5DD-1351-4615-B760-11227F2F14C0}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{7D57F314-9378-4A2D-B066-992AF2C94719}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{7E014B4C-FBD1-48B6-A03D-68D498700E88}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{DA06FB96-C517-4288-838F-DFA74A593612}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F42AFF-70F5-4FDB-9AA4-AB18D142B6B4}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E477B1D-A550-4492-849D-665F02B394EF}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="18.77734375" customWidth="1"/>
+    <col min="1" max="2" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>987123</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="jasonb@gmail.com" xr:uid="{4BF6B43B-AB38-453A-9D63-F2EBDAAC9A6C}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{8565C2BB-551D-403A-866D-E9B24D9F7837}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>